<commit_message>
Estimaion of first week
</commit_message>
<xml_diff>
--- a/Yashar.xlsx
+++ b/Yashar.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YasarAbbas\Desktop\schedule\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64864890-5147-4CB2-BEDB-D50DAE5BB42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD11C68-285F-480B-9474-E1A4DB831F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65ECBCA3-D047-493C-B767-A2AD1CA6521D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{65ECBCA3-D047-493C-B767-A2AD1CA6521D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
-    <sheet name="Result" sheetId="2" r:id="rId2"/>
-    <sheet name="Deutsch" sheetId="3" r:id="rId3"/>
+    <sheet name="Estimation" sheetId="4" r:id="rId2"/>
+    <sheet name="Result" sheetId="2" r:id="rId3"/>
+    <sheet name="Deutsch" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t>Visual Studio Code</t>
   </si>
@@ -261,6 +262,39 @@
   </si>
   <si>
     <t>میان</t>
+  </si>
+  <si>
+    <t>Estimation Date</t>
+  </si>
+  <si>
+    <t>Estimation Description</t>
+  </si>
+  <si>
+    <t>Actual Date</t>
+  </si>
+  <si>
+    <t>Actual Description</t>
+  </si>
+  <si>
+    <t>12.07.2019</t>
+  </si>
+  <si>
+    <t>Complete SOLID Tutorial Serie</t>
+  </si>
+  <si>
+    <t>End of Chapter 2</t>
+  </si>
+  <si>
+    <t>First Zip File</t>
+  </si>
+  <si>
+    <t>4 of them</t>
+  </si>
+  <si>
+    <t>Maven-Life Cycle-J2EE Tools Chain</t>
+  </si>
+  <si>
+    <t>2 Files of Aghdam and 3 lessons of Basic English Vocabulary</t>
   </si>
 </sst>
 </file>
@@ -1904,9 +1938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA6F3BB-9980-47A4-BEF0-98EDDDF63C16}">
   <dimension ref="A1:AG269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E2" sqref="E2:E7"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2943,6 +2977,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB25DB26-49C3-453C-8656-8710C2F9C536}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D8031E-2E06-49F8-AFB9-4F75A7A2A646}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
@@ -3218,7 +3351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D0B588-364B-49F5-B6E1-5CD93766BDA2}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>